<commit_message>
fix unique user with student card
</commit_message>
<xml_diff>
--- a/src/templates/student-import.xlsx
+++ b/src/templates/student-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOURCE CODE\Project\graduation\Backend\webnc\course-management-service\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766A4AA-9018-41F6-A9CF-CBF4090FDFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB44622-9DBB-4F85-A7B9-5DD54C4A2FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>StudentId</t>
   </si>
   <si>
     <t>FullName</t>
+  </si>
+  <si>
+    <t>Trần VĨnh Phúc</t>
+  </si>
+  <si>
+    <t>Võ Đức Huy</t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A2:C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,6 +398,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>20120551</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20120500</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix binding student card
</commit_message>
<xml_diff>
--- a/src/templates/student-import.xlsx
+++ b/src/templates/student-import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOURCE CODE\Project\graduation\Backend\webnc\course-management-service\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NAM_4\WebNangCAO\DOAN\CUOIKI\COURSERVICE\course-service\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB44622-9DBB-4F85-A7B9-5DD54C4A2FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918D1DC0-BF3F-4B9A-B515-4A0648D7C6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4815" yWindow="1455" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>StudentId</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Võ Đức Huy</t>
+  </si>
+  <si>
+    <t>Nguyễn Đăng Khoa</t>
+  </si>
+  <si>
+    <t>Võ Nhất Khanh</t>
+  </si>
+  <si>
+    <t>Nguyễn Quốc Khoa</t>
   </si>
 </sst>
 </file>
@@ -378,19 +387,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20120551</v>
       </c>
@@ -406,12 +415,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20120500</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20120509</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20120507</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20120511</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>